<commit_message>
sore sabtu sebelum ashar
</commit_message>
<xml_diff>
--- a/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari - Desember 2021_Debi Tomika.xlsx
+++ b/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari - Desember 2021_Debi Tomika.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D29552-CB32-4035-9478-B31FD639E747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5BC925-3BFD-4729-8187-F6144E477F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14535" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -906,11 +906,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -927,8 +924,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1213,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H137"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A89" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I94" sqref="I94"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A68" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,16 +1230,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1458,25 +1458,25 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="16" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="4" t="s">
@@ -1484,13 +1484,13 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
       <c r="H20" s="4" t="s">
         <v>17</v>
       </c>
@@ -1522,16 +1522,16 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="20"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
@@ -1561,16 +1561,16 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="20"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
@@ -1627,16 +1627,16 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="20"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="19"/>
     </row>
     <row r="28" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
@@ -1936,16 +1936,16 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="20"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="19"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
@@ -2104,16 +2104,16 @@
       <c r="H52" s="12"/>
     </row>
     <row r="53" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B53" s="19"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="20"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="19"/>
     </row>
     <row r="54" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
@@ -2892,7 +2892,7 @@
       <c r="C83" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D83" s="21" t="s">
+      <c r="D83" s="14" t="s">
         <v>153</v>
       </c>
       <c r="E83" s="9" t="s">
@@ -2946,7 +2946,7 @@
       <c r="C85" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D85" s="21" t="s">
+      <c r="D85" s="14" t="s">
         <v>157</v>
       </c>
       <c r="E85" s="9" t="s">
@@ -3027,7 +3027,7 @@
       <c r="C88" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D88" s="21" t="s">
+      <c r="D88" s="14" t="s">
         <v>162</v>
       </c>
       <c r="E88" s="9" t="s">
@@ -3081,7 +3081,7 @@
       <c r="C90" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D90" s="21" t="s">
+      <c r="D90" s="14" t="s">
         <v>72</v>
       </c>
       <c r="E90" s="9" t="s">
@@ -3207,16 +3207,16 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="18" t="s">
+      <c r="A95" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B95" s="19"/>
-      <c r="C95" s="19"/>
-      <c r="D95" s="19"/>
-      <c r="E95" s="19"/>
-      <c r="F95" s="19"/>
-      <c r="G95" s="19"/>
-      <c r="H95" s="20"/>
+      <c r="B95" s="18"/>
+      <c r="C95" s="18"/>
+      <c r="D95" s="18"/>
+      <c r="E95" s="18"/>
+      <c r="F95" s="18"/>
+      <c r="G95" s="18"/>
+      <c r="H95" s="19"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
@@ -3231,16 +3231,16 @@
       <c r="H96" s="12"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="18" t="s">
+      <c r="A97" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B97" s="19"/>
-      <c r="C97" s="19"/>
-      <c r="D97" s="19"/>
-      <c r="E97" s="19"/>
-      <c r="F97" s="19"/>
-      <c r="G97" s="19"/>
-      <c r="H97" s="20"/>
+      <c r="B97" s="18"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="18"/>
+      <c r="G97" s="18"/>
+      <c r="H97" s="19"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
@@ -3279,15 +3279,15 @@
       <c r="H100" s="12"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="15" t="s">
+      <c r="A101" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B101" s="15"/>
-      <c r="C101" s="15"/>
-      <c r="D101" s="15"/>
-      <c r="E101" s="15"/>
-      <c r="F101" s="15"/>
-      <c r="G101" s="15"/>
+      <c r="B101" s="21"/>
+      <c r="C101" s="21"/>
+      <c r="D101" s="21"/>
+      <c r="E101" s="21"/>
+      <c r="F101" s="21"/>
+      <c r="G101" s="21"/>
       <c r="H101" s="6">
         <f>SUM(H23:H100)</f>
         <v>45.249999999999972</v>
@@ -3311,11 +3311,11 @@
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
-      <c r="F103" s="16" t="s">
+      <c r="F103" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="G103" s="16"/>
-      <c r="H103" s="16"/>
+      <c r="G103" s="15"/>
+      <c r="H103" s="15"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
@@ -3323,11 +3323,11 @@
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
-      <c r="F104" s="16" t="s">
+      <c r="F104" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="G104" s="16"/>
-      <c r="H104" s="16"/>
+      <c r="G104" s="15"/>
+      <c r="H104" s="15"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
@@ -3375,11 +3375,11 @@
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
-      <c r="F109" s="16" t="s">
+      <c r="F109" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="G109" s="16"/>
-      <c r="H109" s="16"/>
+      <c r="G109" s="15"/>
+      <c r="H109" s="15"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
@@ -3387,11 +3387,11 @@
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
-      <c r="F110" s="16" t="s">
+      <c r="F110" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="G110" s="16"/>
-      <c r="H110" s="16"/>
+      <c r="G110" s="15"/>
+      <c r="H110" s="15"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
@@ -3665,12 +3665,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F104:H104"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="A95:H95"/>
-    <mergeCell ref="A22:H22"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A101:G101"/>
     <mergeCell ref="F103:H103"/>
@@ -3685,6 +3679,12 @@
     <mergeCell ref="A53:H53"/>
     <mergeCell ref="A97:H97"/>
     <mergeCell ref="A24:H24"/>
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="A95:H95"/>
+    <mergeCell ref="A22:H22"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
7 Februari 2.30 sore
</commit_message>
<xml_diff>
--- a/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari - Desember 2021_Debi Tomika.xlsx
+++ b/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari - Desember 2021_Debi Tomika.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5BC925-3BFD-4729-8187-F6144E477F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0095D7E6-BCA2-4128-864B-E4DD9360EBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="168">
   <si>
     <t>LAPORAN KEGIATAN PRANATA KOMPUTER</t>
   </si>
@@ -539,18 +539,9 @@
     <t>Melakukan Identifikasi Kebutuhan Pengguna Sistem Informasi Penilaian CKP Pegawai (SICAKEP)</t>
   </si>
   <si>
-    <t>Melakukan Analisis Sistem Informasi Penilaian CKP Pegawai (SICAKEP)</t>
-  </si>
-  <si>
-    <t>III.A.5</t>
-  </si>
-  <si>
     <t>Mei - Juni 2021</t>
   </si>
   <si>
-    <t>Dokumen Hasil Analisis</t>
-  </si>
-  <si>
     <t>Melakukan Pemodelan Proses Sistem Informasi Penilaian CKP Pegawai (SICAKEP)</t>
   </si>
   <si>
@@ -558,9 +549,6 @@
   </si>
   <si>
     <t>Melakukan Identifikasi Kebutuhan Pengguna Sistem Informasi Penilaian Pegawai Terbaik (SIPIA)</t>
-  </si>
-  <si>
-    <t>Melakukan Analisis Sistem Informasi Penilaian Pegawai Terbaik (SIPIA)</t>
   </si>
   <si>
     <t>Menyusun Usulan Pembangunan Sistem Informasi Penilaian Pegawai Terbaik (SIPIA)</t>
@@ -909,6 +897,12 @@
     <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -923,12 +917,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1213,8 +1201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H137"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A68" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A37" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,16 +1218,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1458,25 +1446,25 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="18" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="4" t="s">
@@ -1484,13 +1472,13 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="4" t="s">
         <v>17</v>
       </c>
@@ -1522,16 +1510,16 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
     </row>
     <row r="23" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
@@ -1561,16 +1549,16 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="19"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
@@ -1627,16 +1615,16 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="19"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="21"/>
     </row>
     <row r="28" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
@@ -1936,16 +1924,16 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="19"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="21"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
@@ -2104,16 +2092,16 @@
       <c r="H52" s="12"/>
     </row>
     <row r="53" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="19"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="21"/>
     </row>
     <row r="54" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
@@ -2147,7 +2135,7 @@
         <v>2</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>89</v>
@@ -2201,7 +2189,7 @@
         <v>4</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>93</v>
@@ -2255,7 +2243,7 @@
         <v>6</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>94</v>
@@ -2309,7 +2297,7 @@
         <v>8</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>101</v>
@@ -2331,21 +2319,21 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>9</v>
       </c>
       <c r="B62" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D62" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="C62" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D62" s="13" t="s">
-        <v>102</v>
-      </c>
       <c r="E62" s="9" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F62" s="10">
         <v>0.54</v>
@@ -2354,25 +2342,25 @@
         <v>1</v>
       </c>
       <c r="H62" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="H62:H71" si="10">F62*G62</f>
         <v>0.54</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>10</v>
       </c>
       <c r="B63" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C63" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C63" s="7" t="s">
-        <v>106</v>
-      </c>
       <c r="D63" s="13" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F63" s="10">
         <v>0.54</v>
@@ -2381,7 +2369,7 @@
         <v>1</v>
       </c>
       <c r="H63" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.54</v>
       </c>
     </row>
@@ -2390,26 +2378,24 @@
         <v>11</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C64" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D64" s="13"/>
+      <c r="E64" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="D64" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>117</v>
-      </c>
       <c r="F64" s="10">
-        <v>0.54</v>
+        <v>0.66</v>
       </c>
       <c r="G64" s="11">
         <v>1</v>
       </c>
       <c r="H64" s="12">
-        <f t="shared" si="9"/>
-        <v>0.54</v>
+        <f t="shared" si="10"/>
+        <v>0.66</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
@@ -2417,26 +2403,24 @@
         <v>12</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C65" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D65" s="13"/>
+      <c r="E65" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="D65" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>117</v>
-      </c>
       <c r="F65" s="10">
-        <v>0.54</v>
+        <v>0.66</v>
       </c>
       <c r="G65" s="11">
         <v>1</v>
       </c>
       <c r="H65" s="12">
-        <f t="shared" si="9"/>
-        <v>0.54</v>
+        <f t="shared" si="10"/>
+        <v>0.66</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
@@ -2444,24 +2428,24 @@
         <v>13</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D66" s="13"/>
       <c r="E66" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F66" s="10">
-        <v>0.66</v>
+        <v>0.44</v>
       </c>
       <c r="G66" s="11">
         <v>1</v>
       </c>
       <c r="H66" s="12">
-        <f t="shared" si="9"/>
-        <v>0.66</v>
+        <f t="shared" si="10"/>
+        <v>0.44</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
@@ -2469,24 +2453,24 @@
         <v>14</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D67" s="13"/>
       <c r="E67" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F67" s="10">
-        <v>0.66</v>
+        <v>0.44</v>
       </c>
       <c r="G67" s="11">
         <v>1</v>
       </c>
       <c r="H67" s="12">
-        <f t="shared" si="9"/>
-        <v>0.66</v>
+        <f t="shared" si="10"/>
+        <v>0.44</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
@@ -2494,24 +2478,24 @@
         <v>15</v>
       </c>
       <c r="B68" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C68" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>121</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="9" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F68" s="10">
-        <v>0.44</v>
+        <v>1.21</v>
       </c>
       <c r="G68" s="11">
         <v>1</v>
       </c>
       <c r="H68" s="12">
-        <f t="shared" si="9"/>
-        <v>0.44</v>
+        <f t="shared" si="10"/>
+        <v>1.21</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
@@ -2519,24 +2503,24 @@
         <v>16</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D69" s="13"/>
       <c r="E69" s="9" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F69" s="10">
-        <v>0.44</v>
+        <v>1.21</v>
       </c>
       <c r="G69" s="11">
         <v>1</v>
       </c>
       <c r="H69" s="12">
-        <f t="shared" si="9"/>
-        <v>0.44</v>
+        <f t="shared" si="10"/>
+        <v>1.21</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
@@ -2554,14 +2538,14 @@
         <v>129</v>
       </c>
       <c r="F70" s="10">
-        <v>1.21</v>
+        <v>0.6</v>
       </c>
       <c r="G70" s="11">
         <v>1</v>
       </c>
       <c r="H70" s="12">
-        <f t="shared" si="9"/>
-        <v>1.21</v>
+        <f t="shared" si="10"/>
+        <v>0.6</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
@@ -2579,81 +2563,55 @@
         <v>129</v>
       </c>
       <c r="F71" s="10">
-        <v>1.21</v>
+        <v>0.6</v>
       </c>
       <c r="G71" s="11">
         <v>1</v>
       </c>
       <c r="H71" s="12">
-        <f t="shared" si="9"/>
-        <v>1.21</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="10"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>19</v>
       </c>
-      <c r="B72" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>132</v>
-      </c>
+      <c r="B72" s="8"/>
+      <c r="C72" s="7"/>
       <c r="D72" s="13"/>
-      <c r="E72" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="F72" s="10">
-        <v>0.6</v>
-      </c>
-      <c r="G72" s="11">
-        <v>1</v>
-      </c>
-      <c r="H72" s="12">
-        <f t="shared" si="9"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="E72" s="9"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="12"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>20</v>
       </c>
-      <c r="B73" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>132</v>
-      </c>
+      <c r="B73" s="8"/>
+      <c r="C73" s="7"/>
       <c r="D73" s="13"/>
-      <c r="E73" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="F73" s="10">
-        <v>0.6</v>
-      </c>
-      <c r="G73" s="11">
-        <v>1</v>
-      </c>
-      <c r="H73" s="12">
-        <f t="shared" si="9"/>
-        <v>0.6</v>
-      </c>
+      <c r="E73" s="9"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="12"/>
     </row>
     <row r="74" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <v>21</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F74" s="10">
         <v>0.11</v>
@@ -2671,16 +2629,16 @@
         <v>22</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F75" s="10">
         <v>0.11</v>
@@ -2698,16 +2656,16 @@
         <v>23</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F76" s="10">
         <v>0.11</v>
@@ -2725,16 +2683,16 @@
         <v>24</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F77" s="10">
         <v>0.11</v>
@@ -2752,16 +2710,16 @@
         <v>25</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F78" s="10">
         <v>0.11</v>
@@ -2779,16 +2737,16 @@
         <v>26</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D79" s="13" t="s">
         <v>69</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F79" s="10">
         <v>0.11</v>
@@ -2806,16 +2764,16 @@
         <v>27</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D80" s="13" t="s">
         <v>69</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F80" s="10">
         <v>0.11</v>
@@ -2833,16 +2791,16 @@
         <v>28</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F81" s="10">
         <v>0.11</v>
@@ -2860,16 +2818,16 @@
         <v>29</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F82" s="10">
         <v>0.11</v>
@@ -2887,16 +2845,16 @@
         <v>30</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F83" s="10">
         <v>0.11</v>
@@ -2914,16 +2872,16 @@
         <v>31</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D84" s="13" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F84" s="10">
         <v>0.11</v>
@@ -2941,16 +2899,16 @@
         <v>32</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F85" s="10">
         <v>0.11</v>
@@ -2968,16 +2926,16 @@
         <v>33</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D86" s="13" t="s">
         <v>71</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F86" s="10">
         <v>0.11</v>
@@ -2995,16 +2953,16 @@
         <v>34</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D87" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F87" s="10">
         <v>0.11</v>
@@ -3022,16 +2980,16 @@
         <v>35</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F88" s="10">
         <v>0.11</v>
@@ -3049,16 +3007,16 @@
         <v>36</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D89" s="13" t="s">
         <v>72</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F89" s="10">
         <v>0.11</v>
@@ -3076,16 +3034,16 @@
         <v>37</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D90" s="14" t="s">
         <v>72</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F90" s="10">
         <v>0.11</v>
@@ -3103,16 +3061,16 @@
         <v>38</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D91" s="13" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F91" s="10">
         <v>0.11</v>
@@ -3130,16 +3088,16 @@
         <v>39</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D92" s="13" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F92" s="10">
         <v>0.11</v>
@@ -3157,16 +3115,16 @@
         <v>40</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D93" s="13" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F93" s="10">
         <v>0.11</v>
@@ -3184,16 +3142,16 @@
         <v>41</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D94" s="13" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F94" s="10">
         <v>0.11</v>
@@ -3207,16 +3165,16 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="17" t="s">
+      <c r="A95" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B95" s="18"/>
-      <c r="C95" s="18"/>
-      <c r="D95" s="18"/>
-      <c r="E95" s="18"/>
-      <c r="F95" s="18"/>
-      <c r="G95" s="18"/>
-      <c r="H95" s="19"/>
+      <c r="B95" s="20"/>
+      <c r="C95" s="20"/>
+      <c r="D95" s="20"/>
+      <c r="E95" s="20"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="20"/>
+      <c r="H95" s="21"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
@@ -3231,16 +3189,16 @@
       <c r="H96" s="12"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="17" t="s">
+      <c r="A97" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B97" s="18"/>
-      <c r="C97" s="18"/>
-      <c r="D97" s="18"/>
-      <c r="E97" s="18"/>
-      <c r="F97" s="18"/>
-      <c r="G97" s="18"/>
-      <c r="H97" s="19"/>
+      <c r="B97" s="20"/>
+      <c r="C97" s="20"/>
+      <c r="D97" s="20"/>
+      <c r="E97" s="20"/>
+      <c r="F97" s="20"/>
+      <c r="G97" s="20"/>
+      <c r="H97" s="21"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
@@ -3279,18 +3237,18 @@
       <c r="H100" s="12"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="21" t="s">
+      <c r="A101" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B101" s="21"/>
-      <c r="C101" s="21"/>
-      <c r="D101" s="21"/>
-      <c r="E101" s="21"/>
-      <c r="F101" s="21"/>
-      <c r="G101" s="21"/>
+      <c r="B101" s="16"/>
+      <c r="C101" s="16"/>
+      <c r="D101" s="16"/>
+      <c r="E101" s="16"/>
+      <c r="F101" s="16"/>
+      <c r="G101" s="16"/>
       <c r="H101" s="6">
         <f>SUM(H23:H100)</f>
-        <v>45.249999999999972</v>
+        <v>44.169999999999973</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -3311,11 +3269,11 @@
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
-      <c r="F103" s="15" t="s">
+      <c r="F103" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="G103" s="15"/>
-      <c r="H103" s="15"/>
+      <c r="G103" s="17"/>
+      <c r="H103" s="17"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
@@ -3323,11 +3281,11 @@
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
-      <c r="F104" s="15" t="s">
+      <c r="F104" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="G104" s="15"/>
-      <c r="H104" s="15"/>
+      <c r="G104" s="17"/>
+      <c r="H104" s="17"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
@@ -3375,11 +3333,11 @@
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
-      <c r="F109" s="15" t="s">
+      <c r="F109" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="G109" s="15"/>
-      <c r="H109" s="15"/>
+      <c r="G109" s="17"/>
+      <c r="H109" s="17"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
@@ -3387,11 +3345,11 @@
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
-      <c r="F110" s="15" t="s">
+      <c r="F110" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="G110" s="15"/>
-      <c r="H110" s="15"/>
+      <c r="G110" s="17"/>
+      <c r="H110" s="17"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
@@ -3665,6 +3623,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="A95:H95"/>
+    <mergeCell ref="A22:H22"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A101:G101"/>
     <mergeCell ref="F103:H103"/>
@@ -3679,12 +3643,6 @@
     <mergeCell ref="A53:H53"/>
     <mergeCell ref="A97:H97"/>
     <mergeCell ref="A24:H24"/>
-    <mergeCell ref="F104:H104"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="A95:H95"/>
-    <mergeCell ref="A22:H22"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
14 maret 2023, sebelum zuhur
</commit_message>
<xml_diff>
--- a/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari - Desember 2021_Debi Tomika.xlsx
+++ b/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari - Desember 2021_Debi Tomika.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0095D7E6-BCA2-4128-864B-E4DD9360EBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA71A1EF-A73D-432C-B73F-9EE7AF48A2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -497,12 +497,6 @@
     <t>Jan - Mar 2021</t>
   </si>
   <si>
-    <t>Menyusun Usulan Pembangunan Sistem Informasi Penilaian CKP Pegawai (SICAKEP)</t>
-  </si>
-  <si>
-    <t>Menyusun Rencana Studi Kelayakan Sistem Informasi Penilaian CKP Pegawai (SICAKEP)</t>
-  </si>
-  <si>
     <t>III.A.2</t>
   </si>
   <si>
@@ -515,9 +509,6 @@
     <t>Proposal Rencana Studi</t>
   </si>
   <si>
-    <t>Melakukan Studi Kelayakan Sistem Informasi Penilaian CKP Pegawai (SICAKEP)</t>
-  </si>
-  <si>
     <t>April 2021</t>
   </si>
   <si>
@@ -536,15 +527,9 @@
     <t>Dokumen Hasil Identifikasi</t>
   </si>
   <si>
-    <t>Melakukan Identifikasi Kebutuhan Pengguna Sistem Informasi Penilaian CKP Pegawai (SICAKEP)</t>
-  </si>
-  <si>
     <t>Mei - Juni 2021</t>
   </si>
   <si>
-    <t>Melakukan Pemodelan Proses Sistem Informasi Penilaian CKP Pegawai (SICAKEP)</t>
-  </si>
-  <si>
     <t>Melakukan Pemodelan Proses Sistem Informasi Penilaian Pegawai Terbaik (SIPIA)</t>
   </si>
   <si>
@@ -566,9 +551,6 @@
     <t>Dokumen Hasil Pemodelan</t>
   </si>
   <si>
-    <t>Melakukan Perancangan Sistem Informasi Penilaian CKP Pegawai (SICAKEP)</t>
-  </si>
-  <si>
     <t>III.A.7</t>
   </si>
   <si>
@@ -584,15 +566,9 @@
     <t>Melakukan Perancangan Sistem Informasi Penilaian Pegawai Terbaik (SIPIA)</t>
   </si>
   <si>
-    <t>Membuat Algoritma Pemrograman Sistem Informasi Penilaian CKP Pegawai (SICAKEP)</t>
-  </si>
-  <si>
     <t>Membuat Algoritma Pemrograman  Sistem Informasi Penilaian Pegawai Terbaik (SIPIA)</t>
   </si>
   <si>
-    <t>Membuat Program Aplikasi Sistem Informasi Penilaian CKP Pegawai (SICAKEP)</t>
-  </si>
-  <si>
     <t>Membuat Program Aplikasi Sistem Informasi Penilaian Pegawai Terbaik (SIPIA)</t>
   </si>
   <si>
@@ -602,9 +578,6 @@
     <t>Program Aplikasi</t>
   </si>
   <si>
-    <t>Mengembangkan Program Aplikasi Sistem Informasi Penilaian CKP Pegawai (SICAKEP)</t>
-  </si>
-  <si>
     <t>Mengembangkan Program Aplikasi Sistem Informasi Penilaian Pegawai Terbaik (SIPIA)</t>
   </si>
   <si>
@@ -726,6 +699,33 @@
   </si>
   <si>
     <t>27 Oktober 2021</t>
+  </si>
+  <si>
+    <t>Menyusun Usulan Pembangunan Sistem Informasi Penilaian Capaian Kinerja Pegawai (SICAKEP)</t>
+  </si>
+  <si>
+    <t>Menyusun Rencana Studi Kelayakan Sistem Informasi Penilaian Capaian Kinerja Pegawai (SICAKEP)</t>
+  </si>
+  <si>
+    <t>Melakukan Studi Kelayakan Sistem Informasi Penilaian Capaian Kinerja Pegawai (SICAKEP)</t>
+  </si>
+  <si>
+    <t>Melakukan Identifikasi Kebutuhan Pengguna Sistem Informasi Penilaian Capaian Kinerja Pegawai (SICAKEP)</t>
+  </si>
+  <si>
+    <t>Melakukan Pemodelan Proses Sistem Informasi Penilaian Capaian Kinerja Pegawai (SICAKEP)</t>
+  </si>
+  <si>
+    <t>Melakukan Perancangan Sistem Informasi Penilaian Capaian Kinerja Pegawai (SICAKEP)</t>
+  </si>
+  <si>
+    <t>Membuat Algoritma Pemrograman Sistem Informasi Penilaian Capaian Kinerja Pegawai (SICAKEP)</t>
+  </si>
+  <si>
+    <t>Membuat Program Aplikasi Sistem Informasi Penilaian Capaian Kinerja Pegawai (SICAKEP)</t>
+  </si>
+  <si>
+    <t>Mengembangkan Program Aplikasi Sistem Informasi Penilaian Capaian Kinerja Pegawai (SICAKEP)</t>
   </si>
 </sst>
 </file>
@@ -897,12 +897,6 @@
     <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -917,6 +911,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1201,8 +1201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H137"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A37" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A49" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,16 +1218,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1446,25 +1446,25 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="16" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="4" t="s">
@@ -1472,13 +1472,13 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
       <c r="H20" s="4" t="s">
         <v>17</v>
       </c>
@@ -1510,16 +1510,16 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="21"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
@@ -1549,16 +1549,16 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="21"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
@@ -1615,16 +1615,16 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="21"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="19"/>
     </row>
     <row r="28" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
@@ -1924,16 +1924,16 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="21"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="19"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
@@ -2092,23 +2092,23 @@
       <c r="H52" s="12"/>
     </row>
     <row r="53" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="21"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="19"/>
     </row>
     <row r="54" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>1</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>91</v>
+        <v>159</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>89</v>
@@ -2117,7 +2117,7 @@
         <v>90</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F54" s="10">
         <v>0.88</v>
@@ -2135,7 +2135,7 @@
         <v>2</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>89</v>
@@ -2144,7 +2144,7 @@
         <v>90</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F55" s="10">
         <v>0.88</v>
@@ -2162,16 +2162,16 @@
         <v>3</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>92</v>
+        <v>160</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D56" s="13" t="s">
         <v>90</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F56" s="10">
         <v>0.22</v>
@@ -2189,16 +2189,16 @@
         <v>4</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D57" s="13" t="s">
         <v>90</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F57" s="10">
         <v>0.22</v>
@@ -2216,16 +2216,16 @@
         <v>5</v>
       </c>
       <c r="B58" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E58" s="9" t="s">
         <v>97</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>100</v>
       </c>
       <c r="F58" s="10">
         <v>0.44</v>
@@ -2243,16 +2243,16 @@
         <v>6</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F59" s="10">
         <v>0.44</v>
@@ -2270,16 +2270,16 @@
         <v>7</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>104</v>
+        <v>162</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F60" s="10">
         <v>0.55000000000000004</v>
@@ -2297,16 +2297,16 @@
         <v>8</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F61" s="10">
         <v>0.55000000000000004</v>
@@ -2324,16 +2324,16 @@
         <v>9</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>106</v>
+        <v>163</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F62" s="10">
         <v>0.54</v>
@@ -2351,16 +2351,16 @@
         <v>10</v>
       </c>
       <c r="B63" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C63" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C63" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="D63" s="13" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F63" s="10">
         <v>0.54</v>
@@ -2378,14 +2378,14 @@
         <v>11</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>114</v>
+        <v>164</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D64" s="13"/>
       <c r="E64" s="9" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F64" s="10">
         <v>0.66</v>
@@ -2403,14 +2403,14 @@
         <v>12</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D65" s="13"/>
       <c r="E65" s="9" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F65" s="10">
         <v>0.66</v>
@@ -2428,14 +2428,14 @@
         <v>13</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>120</v>
+        <v>165</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D66" s="13"/>
       <c r="E66" s="9" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F66" s="10">
         <v>0.44</v>
@@ -2453,14 +2453,14 @@
         <v>14</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D67" s="13"/>
       <c r="E67" s="9" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F67" s="10">
         <v>0.44</v>
@@ -2478,14 +2478,14 @@
         <v>15</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>122</v>
+        <v>166</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="9" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F68" s="10">
         <v>1.21</v>
@@ -2503,14 +2503,14 @@
         <v>16</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D69" s="13"/>
       <c r="E69" s="9" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F69" s="10">
         <v>1.21</v>
@@ -2528,14 +2528,14 @@
         <v>17</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>126</v>
+        <v>167</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="9" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F70" s="10">
         <v>0.6</v>
@@ -2553,14 +2553,14 @@
         <v>18</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="9" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F71" s="10">
         <v>0.6</v>
@@ -2602,16 +2602,16 @@
         <v>21</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F74" s="10">
         <v>0.11</v>
@@ -2629,16 +2629,16 @@
         <v>22</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F75" s="10">
         <v>0.11</v>
@@ -2656,16 +2656,16 @@
         <v>23</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F76" s="10">
         <v>0.11</v>
@@ -2683,16 +2683,16 @@
         <v>24</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F77" s="10">
         <v>0.11</v>
@@ -2710,16 +2710,16 @@
         <v>25</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F78" s="10">
         <v>0.11</v>
@@ -2737,16 +2737,16 @@
         <v>26</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D79" s="13" t="s">
         <v>69</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F79" s="10">
         <v>0.11</v>
@@ -2764,16 +2764,16 @@
         <v>27</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D80" s="13" t="s">
         <v>69</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F80" s="10">
         <v>0.11</v>
@@ -2791,16 +2791,16 @@
         <v>28</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F81" s="10">
         <v>0.11</v>
@@ -2818,16 +2818,16 @@
         <v>29</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F82" s="10">
         <v>0.11</v>
@@ -2845,16 +2845,16 @@
         <v>30</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F83" s="10">
         <v>0.11</v>
@@ -2872,16 +2872,16 @@
         <v>31</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D84" s="13" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F84" s="10">
         <v>0.11</v>
@@ -2899,16 +2899,16 @@
         <v>32</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F85" s="10">
         <v>0.11</v>
@@ -2926,16 +2926,16 @@
         <v>33</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D86" s="13" t="s">
         <v>71</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F86" s="10">
         <v>0.11</v>
@@ -2953,16 +2953,16 @@
         <v>34</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D87" s="13" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F87" s="10">
         <v>0.11</v>
@@ -2980,16 +2980,16 @@
         <v>35</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F88" s="10">
         <v>0.11</v>
@@ -3007,16 +3007,16 @@
         <v>36</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D89" s="13" t="s">
         <v>72</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F89" s="10">
         <v>0.11</v>
@@ -3034,16 +3034,16 @@
         <v>37</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D90" s="14" t="s">
         <v>72</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F90" s="10">
         <v>0.11</v>
@@ -3061,16 +3061,16 @@
         <v>38</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D91" s="13" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F91" s="10">
         <v>0.11</v>
@@ -3088,16 +3088,16 @@
         <v>39</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D92" s="13" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F92" s="10">
         <v>0.11</v>
@@ -3115,16 +3115,16 @@
         <v>40</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D93" s="13" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E93" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F93" s="10">
         <v>0.11</v>
@@ -3142,16 +3142,16 @@
         <v>41</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D94" s="13" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F94" s="10">
         <v>0.11</v>
@@ -3165,16 +3165,16 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="19" t="s">
+      <c r="A95" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B95" s="20"/>
-      <c r="C95" s="20"/>
-      <c r="D95" s="20"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="20"/>
-      <c r="G95" s="20"/>
-      <c r="H95" s="21"/>
+      <c r="B95" s="18"/>
+      <c r="C95" s="18"/>
+      <c r="D95" s="18"/>
+      <c r="E95" s="18"/>
+      <c r="F95" s="18"/>
+      <c r="G95" s="18"/>
+      <c r="H95" s="19"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
@@ -3189,16 +3189,16 @@
       <c r="H96" s="12"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="19" t="s">
+      <c r="A97" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B97" s="20"/>
-      <c r="C97" s="20"/>
-      <c r="D97" s="20"/>
-      <c r="E97" s="20"/>
-      <c r="F97" s="20"/>
-      <c r="G97" s="20"/>
-      <c r="H97" s="21"/>
+      <c r="B97" s="18"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="18"/>
+      <c r="G97" s="18"/>
+      <c r="H97" s="19"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
@@ -3237,15 +3237,15 @@
       <c r="H100" s="12"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="16" t="s">
+      <c r="A101" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B101" s="16"/>
-      <c r="C101" s="16"/>
-      <c r="D101" s="16"/>
-      <c r="E101" s="16"/>
-      <c r="F101" s="16"/>
-      <c r="G101" s="16"/>
+      <c r="B101" s="21"/>
+      <c r="C101" s="21"/>
+      <c r="D101" s="21"/>
+      <c r="E101" s="21"/>
+      <c r="F101" s="21"/>
+      <c r="G101" s="21"/>
       <c r="H101" s="6">
         <f>SUM(H23:H100)</f>
         <v>44.169999999999973</v>
@@ -3269,11 +3269,11 @@
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
-      <c r="F103" s="17" t="s">
+      <c r="F103" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="G103" s="17"/>
-      <c r="H103" s="17"/>
+      <c r="G103" s="15"/>
+      <c r="H103" s="15"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
@@ -3281,11 +3281,11 @@
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
-      <c r="F104" s="17" t="s">
+      <c r="F104" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="G104" s="17"/>
-      <c r="H104" s="17"/>
+      <c r="G104" s="15"/>
+      <c r="H104" s="15"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
@@ -3333,11 +3333,11 @@
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
-      <c r="F109" s="17" t="s">
+      <c r="F109" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="G109" s="17"/>
-      <c r="H109" s="17"/>
+      <c r="G109" s="15"/>
+      <c r="H109" s="15"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
@@ -3345,11 +3345,11 @@
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
-      <c r="F110" s="17" t="s">
+      <c r="F110" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="G110" s="17"/>
-      <c r="H110" s="17"/>
+      <c r="G110" s="15"/>
+      <c r="H110" s="15"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
@@ -3623,12 +3623,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F104:H104"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="A95:H95"/>
-    <mergeCell ref="A22:H22"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A101:G101"/>
     <mergeCell ref="F103:H103"/>
@@ -3643,6 +3637,12 @@
     <mergeCell ref="A53:H53"/>
     <mergeCell ref="A97:H97"/>
     <mergeCell ref="A24:H24"/>
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="A95:H95"/>
+    <mergeCell ref="A22:H22"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
18 maret, malam sebelum tidur
</commit_message>
<xml_diff>
--- a/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari - Desember 2021_Debi Tomika.xlsx
+++ b/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari - Desember 2021_Debi Tomika.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA71A1EF-A73D-432C-B73F-9EE7AF48A2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEAF845-15F5-45B5-9EA9-E5E03372031A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -897,6 +908,12 @@
     <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -911,12 +928,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1199,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H137"/>
+  <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A49" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A76" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="G90" sqref="G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,16 +1229,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1446,25 +1457,25 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="18" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="4" t="s">
@@ -1472,13 +1483,13 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="4" t="s">
         <v>17</v>
       </c>
@@ -1510,16 +1521,16 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
     </row>
     <row r="23" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
@@ -1549,16 +1560,16 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="19"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
@@ -1615,16 +1626,16 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="19"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="21"/>
     </row>
     <row r="28" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
@@ -1924,16 +1935,16 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="19"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="21"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
@@ -2092,16 +2103,16 @@
       <c r="H52" s="12"/>
     </row>
     <row r="53" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="19"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="21"/>
     </row>
     <row r="54" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
@@ -2126,7 +2137,7 @@
         <v>1</v>
       </c>
       <c r="H54" s="12">
-        <f t="shared" ref="H54:H94" si="9">F54*G54</f>
+        <f t="shared" ref="H54:H92" si="9">F54*G54</f>
         <v>0.88</v>
       </c>
     </row>
@@ -2573,42 +2584,72 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>19</v>
       </c>
-      <c r="B72" s="8"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="9"/>
-      <c r="F72" s="10"/>
-      <c r="G72" s="11"/>
-      <c r="H72" s="12"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D72" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F72" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G72" s="11">
+        <v>1</v>
+      </c>
+      <c r="H72" s="12">
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>20</v>
       </c>
-      <c r="B73" s="8"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="10"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="12"/>
+      <c r="B73" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D73" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F73" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G73" s="11">
+        <v>1</v>
+      </c>
+      <c r="H73" s="12">
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
     </row>
     <row r="74" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <v>21</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="E74" s="9" t="s">
         <v>124</v>
@@ -2629,13 +2670,13 @@
         <v>22</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E75" s="9" t="s">
         <v>124</v>
@@ -2656,13 +2697,13 @@
         <v>23</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E76" s="9" t="s">
         <v>124</v>
@@ -2678,18 +2719,18 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
         <v>24</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>129</v>
+        <v>69</v>
       </c>
       <c r="E77" s="9" t="s">
         <v>124</v>
@@ -2710,13 +2751,13 @@
         <v>25</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>132</v>
+        <v>69</v>
       </c>
       <c r="E78" s="9" t="s">
         <v>124</v>
@@ -2732,18 +2773,18 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <v>26</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>69</v>
+        <v>135</v>
       </c>
       <c r="E79" s="9" t="s">
         <v>124</v>
@@ -2764,13 +2805,13 @@
         <v>27</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>69</v>
+        <v>139</v>
       </c>
       <c r="E80" s="9" t="s">
         <v>124</v>
@@ -2786,18 +2827,18 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <v>28</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D81" s="13" t="s">
-        <v>135</v>
+      <c r="D81" s="14" t="s">
+        <v>140</v>
       </c>
       <c r="E81" s="9" t="s">
         <v>124</v>
@@ -2818,13 +2859,13 @@
         <v>29</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E82" s="9" t="s">
         <v>124</v>
@@ -2845,13 +2886,13 @@
         <v>30</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E83" s="9" t="s">
         <v>124</v>
@@ -2872,13 +2913,13 @@
         <v>31</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D84" s="13" t="s">
-        <v>142</v>
+        <v>71</v>
       </c>
       <c r="E84" s="9" t="s">
         <v>124</v>
@@ -2899,13 +2940,13 @@
         <v>32</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D85" s="14" t="s">
-        <v>144</v>
+      <c r="D85" s="13" t="s">
+        <v>147</v>
       </c>
       <c r="E85" s="9" t="s">
         <v>124</v>
@@ -2926,13 +2967,13 @@
         <v>33</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D86" s="13" t="s">
-        <v>71</v>
+      <c r="D86" s="14" t="s">
+        <v>149</v>
       </c>
       <c r="E86" s="9" t="s">
         <v>124</v>
@@ -2948,18 +2989,18 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
         <v>34</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D87" s="13" t="s">
-        <v>147</v>
+        <v>72</v>
       </c>
       <c r="E87" s="9" t="s">
         <v>124</v>
@@ -2980,13 +3021,13 @@
         <v>35</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>149</v>
+        <v>72</v>
       </c>
       <c r="E88" s="9" t="s">
         <v>124</v>
@@ -3002,18 +3043,18 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
         <v>36</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C89" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D89" s="13" t="s">
-        <v>72</v>
+        <v>153</v>
       </c>
       <c r="E89" s="9" t="s">
         <v>124</v>
@@ -3029,18 +3070,18 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
         <v>37</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D90" s="14" t="s">
-        <v>72</v>
+      <c r="D90" s="13" t="s">
+        <v>155</v>
       </c>
       <c r="E90" s="9" t="s">
         <v>124</v>
@@ -3061,13 +3102,13 @@
         <v>38</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D91" s="13" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E91" s="9" t="s">
         <v>124</v>
@@ -3083,18 +3124,18 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A92" s="7">
         <v>39</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D92" s="13" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E92" s="9" t="s">
         <v>124</v>
@@ -3110,71 +3151,41 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="57" x14ac:dyDescent="0.25">
-      <c r="A93" s="7">
-        <v>40</v>
-      </c>
-      <c r="B93" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D93" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F93" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="G93" s="11">
-        <v>1</v>
-      </c>
-      <c r="H93" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B93" s="20"/>
+      <c r="C93" s="20"/>
+      <c r="D93" s="20"/>
+      <c r="E93" s="20"/>
+      <c r="F93" s="20"/>
+      <c r="G93" s="20"/>
+      <c r="H93" s="21"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="7">
-        <v>41</v>
-      </c>
-      <c r="B94" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D94" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F94" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="G94" s="11">
-        <v>1</v>
-      </c>
-      <c r="H94" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B95" s="18"/>
-      <c r="C95" s="18"/>
-      <c r="D95" s="18"/>
-      <c r="E95" s="18"/>
-      <c r="F95" s="18"/>
-      <c r="G95" s="18"/>
-      <c r="H95" s="19"/>
+        <v>1</v>
+      </c>
+      <c r="B94" s="8"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="10"/>
+      <c r="G94" s="11"/>
+      <c r="H94" s="12"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B95" s="20"/>
+      <c r="C95" s="20"/>
+      <c r="D95" s="20"/>
+      <c r="E95" s="20"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="20"/>
+      <c r="H95" s="21"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
@@ -3189,20 +3200,20 @@
       <c r="H96" s="12"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B97" s="18"/>
-      <c r="C97" s="18"/>
-      <c r="D97" s="18"/>
-      <c r="E97" s="18"/>
-      <c r="F97" s="18"/>
-      <c r="G97" s="18"/>
-      <c r="H97" s="19"/>
+      <c r="A97" s="7">
+        <v>2</v>
+      </c>
+      <c r="B97" s="8"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="13"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="10"/>
+      <c r="G97" s="11"/>
+      <c r="H97" s="12"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B98" s="8"/>
       <c r="C98" s="7"/>
@@ -3213,55 +3224,55 @@
       <c r="H98" s="12"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="7">
-        <v>2</v>
-      </c>
-      <c r="B99" s="8"/>
-      <c r="C99" s="7"/>
-      <c r="D99" s="13"/>
-      <c r="E99" s="9"/>
-      <c r="F99" s="10"/>
-      <c r="G99" s="11"/>
-      <c r="H99" s="12"/>
+      <c r="A99" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B99" s="16"/>
+      <c r="C99" s="16"/>
+      <c r="D99" s="16"/>
+      <c r="E99" s="16"/>
+      <c r="F99" s="16"/>
+      <c r="G99" s="16"/>
+      <c r="H99" s="6">
+        <f>SUM(H23:H98)</f>
+        <v>44.169999999999973</v>
+      </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="7">
-        <v>3</v>
-      </c>
-      <c r="B100" s="8"/>
-      <c r="C100" s="7"/>
-      <c r="D100" s="13"/>
-      <c r="E100" s="9"/>
-      <c r="F100" s="10"/>
-      <c r="G100" s="11"/>
-      <c r="H100" s="12"/>
+      <c r="A100" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B100" s="2"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B101" s="21"/>
-      <c r="C101" s="21"/>
-      <c r="D101" s="21"/>
-      <c r="E101" s="21"/>
-      <c r="F101" s="21"/>
-      <c r="G101" s="21"/>
-      <c r="H101" s="6">
-        <f>SUM(H23:H100)</f>
-        <v>44.169999999999973</v>
-      </c>
+      <c r="A101" s="1"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G101" s="17"/>
+      <c r="H101" s="17"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="A102" s="1"/>
       <c r="B102" s="2"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
-      <c r="G102" s="1"/>
-      <c r="H102" s="1"/>
+      <c r="F102" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G102" s="17"/>
+      <c r="H102" s="17"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
@@ -3269,11 +3280,9 @@
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
-      <c r="F103" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="G103" s="15"/>
-      <c r="H103" s="15"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
@@ -3281,11 +3290,9 @@
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
-      <c r="F104" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G104" s="15"/>
-      <c r="H104" s="15"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
@@ -3313,9 +3320,11 @@
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
-      <c r="F107" s="1"/>
-      <c r="G107" s="1"/>
-      <c r="H107" s="1"/>
+      <c r="F107" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G107" s="17"/>
+      <c r="H107" s="17"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
@@ -3323,9 +3332,11 @@
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
-      <c r="F108" s="1"/>
-      <c r="G108" s="1"/>
-      <c r="H108" s="1"/>
+      <c r="F108" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G108" s="17"/>
+      <c r="H108" s="17"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
@@ -3333,11 +3344,9 @@
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
-      <c r="F109" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="G109" s="15"/>
-      <c r="H109" s="15"/>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
@@ -3345,11 +3354,9 @@
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
-      <c r="F110" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="G110" s="15"/>
-      <c r="H110" s="15"/>
+      <c r="F110" s="1"/>
+      <c r="G110" s="1"/>
+      <c r="H110" s="1"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
@@ -3601,31 +3608,17 @@
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A136" s="1"/>
-      <c r="B136" s="2"/>
-      <c r="C136" s="1"/>
-      <c r="D136" s="1"/>
-      <c r="E136" s="1"/>
-      <c r="F136" s="1"/>
-      <c r="G136" s="1"/>
-      <c r="H136" s="1"/>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A137" s="1"/>
-      <c r="B137" s="2"/>
-      <c r="C137" s="1"/>
-      <c r="D137" s="1"/>
-      <c r="E137" s="1"/>
-      <c r="F137" s="1"/>
-      <c r="G137" s="1"/>
-      <c r="H137" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="A93:H93"/>
+    <mergeCell ref="A22:H22"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A101:G101"/>
-    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="A99:G99"/>
+    <mergeCell ref="F101:H101"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
@@ -3635,14 +3628,8 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="A39:H39"/>
     <mergeCell ref="A53:H53"/>
-    <mergeCell ref="A97:H97"/>
+    <mergeCell ref="A95:H95"/>
     <mergeCell ref="A24:H24"/>
-    <mergeCell ref="F104:H104"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="A95:H95"/>
-    <mergeCell ref="A22:H22"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
19 maret sebelum tidur
</commit_message>
<xml_diff>
--- a/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari - Desember 2021_Debi Tomika.xlsx
+++ b/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari - Desember 2021_Debi Tomika.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEAF845-15F5-45B5-9EA9-E5E03372031A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B6DA19-3934-413E-A6A8-A458221E498F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,23 +15,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="182">
   <si>
     <t>LAPORAN KEGIATAN PRANATA KOMPUTER</t>
   </si>
@@ -589,15 +578,6 @@
     <t>Program Aplikasi</t>
   </si>
   <si>
-    <t>Mengembangkan Program Aplikasi Sistem Informasi Penilaian Pegawai Terbaik (SIPIA)</t>
-  </si>
-  <si>
-    <t>III.A.10</t>
-  </si>
-  <si>
-    <t>Dokumentasi</t>
-  </si>
-  <si>
     <t>Instalasi Program Entri Data Updating SAKERNAS Februari 2021 (Versi P21Feb.1) di Pusat Olah BPS Kabupaten Kuantan Singingi</t>
   </si>
   <si>
@@ -736,7 +716,121 @@
     <t>Membuat Program Aplikasi Sistem Informasi Penilaian Capaian Kinerja Pegawai (SICAKEP)</t>
   </si>
   <si>
-    <t>Mengembangkan Program Aplikasi Sistem Informasi Penilaian Capaian Kinerja Pegawai (SICAKEP)</t>
+    <t>III.A.11</t>
+  </si>
+  <si>
+    <t>Dokumen Rule Validasi</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Menyusun Definisi </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Rule</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Validasi Sistem Informasi Penilaian Capaian Kinerja Pegawai (SICAKEP)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Menyusun Definisi </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Rule</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Validasi  Sistem Informasi Penilaian Pegawai Terbaik (SIPIA)</t>
+    </r>
+  </si>
+  <si>
+    <t>III.A.17</t>
+  </si>
+  <si>
+    <t>Buku Petunjuk Operasional</t>
+  </si>
+  <si>
+    <t>Menyusun Petunjuk Operasional Sistem Informasi Penilaian Capaian Kinerja Pegawai (SICAKEP)</t>
+  </si>
+  <si>
+    <t>Menyusun Petunjuk Operasional Sistem Informasi Penilaian Pegawai Terbaik (SIPIA)</t>
+  </si>
+  <si>
+    <t>Menyusun Usulan Pembangunan Sistem Informasi Desa Cinta Statistik (SICANTIK)</t>
+  </si>
+  <si>
+    <t>Menyusun Rencana Studi Kelayakan Sistem Informasi Desa Cinta Statistik (SICANTIK)</t>
+  </si>
+  <si>
+    <t>Melakukan Studi Kelayakan Sistem Informasi Desa Cinta Statistik (SICANTIK)</t>
+  </si>
+  <si>
+    <t>Melakukan Identifikasi Kebutuhan Pengguna Sistem Informasi Desa Cinta Statistik (SICANTIK)</t>
+  </si>
+  <si>
+    <t>Melakukan Pemodelan Proses Sistem Informasi Desa Cinta Statistik (SICANTIK)</t>
+  </si>
+  <si>
+    <t>Melakukan Perancangan Sistem Informasi Desa Cinta Statistik (SICANTIK)</t>
+  </si>
+  <si>
+    <t>Membuat Algoritma Pemrograman Sistem Informasi Desa Cinta Statistik (SICANTIK)</t>
+  </si>
+  <si>
+    <t>Membuat Program Aplikasi Sistem Informasi Desa Cinta Statistik (SICANTIK)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Menyusun Definisi </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Rule</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Validasi Sistem Informasi Desa Cinta Statistik (SICANTIK)</t>
+    </r>
+  </si>
+  <si>
+    <t>Menyusun Petunjuk Operasional Sistem Informasi Desa Cinta Statistik (SICANTIK)</t>
   </si>
 </sst>
 </file>
@@ -1210,10 +1304,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H135"/>
+  <dimension ref="A1:H147"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A76" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="G90" sqref="G90"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A90" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2119,7 +2213,7 @@
         <v>1</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>89</v>
@@ -2137,7 +2231,7 @@
         <v>1</v>
       </c>
       <c r="H54" s="12">
-        <f t="shared" ref="H54:H92" si="9">F54*G54</f>
+        <f t="shared" ref="H54:H94" si="9">F54*G54</f>
         <v>0.88</v>
       </c>
     </row>
@@ -2173,7 +2267,7 @@
         <v>3</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>91</v>
@@ -2227,7 +2321,7 @@
         <v>5</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>92</v>
@@ -2281,7 +2375,7 @@
         <v>7</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>98</v>
@@ -2335,7 +2429,7 @@
         <v>9</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>107</v>
@@ -2389,7 +2483,7 @@
         <v>11</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>109</v>
@@ -2439,7 +2533,7 @@
         <v>13</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>111</v>
@@ -2489,7 +2583,7 @@
         <v>15</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>116</v>
@@ -2539,24 +2633,24 @@
         <v>17</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>119</v>
+        <v>164</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="9" t="s">
-        <v>120</v>
+        <v>165</v>
       </c>
       <c r="F70" s="10">
-        <v>0.6</v>
+        <v>0.44</v>
       </c>
       <c r="G70" s="11">
         <v>1</v>
       </c>
       <c r="H70" s="12">
         <f t="shared" si="10"/>
-        <v>0.6</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
@@ -2564,78 +2658,74 @@
         <v>18</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>118</v>
+        <v>167</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>119</v>
+        <v>164</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="9" t="s">
-        <v>120</v>
+        <v>165</v>
       </c>
       <c r="F71" s="10">
-        <v>0.6</v>
+        <v>0.44</v>
       </c>
       <c r="G71" s="11">
         <v>1</v>
       </c>
       <c r="H71" s="12">
         <f t="shared" si="10"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>19</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>121</v>
+        <v>170</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D72" s="13" t="s">
-        <v>123</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="D72" s="13"/>
       <c r="E72" s="9" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="F72" s="10">
-        <v>0.11</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="G72" s="11">
         <v>1</v>
       </c>
       <c r="H72" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H72:H73" si="11">F72*G72</f>
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>20</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>127</v>
+        <v>171</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D73" s="13" t="s">
-        <v>125</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="D73" s="13"/>
       <c r="E73" s="9" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="F73" s="10">
-        <v>0.11</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="G73" s="11">
         <v>1</v>
       </c>
       <c r="H73" s="12">
-        <f t="shared" si="9"/>
-        <v>0.11</v>
+        <f t="shared" si="11"/>
+        <v>0.16500000000000001</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="57" x14ac:dyDescent="0.25">
@@ -2643,16 +2733,16 @@
         <v>21</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F74" s="10">
         <v>0.11</v>
@@ -2670,16 +2760,16 @@
         <v>22</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C75" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D75" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D75" s="13" t="s">
-        <v>129</v>
-      </c>
       <c r="E75" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F75" s="10">
         <v>0.11</v>
@@ -2697,16 +2787,16 @@
         <v>23</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F76" s="10">
         <v>0.11</v>
@@ -2719,21 +2809,21 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
         <v>24</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>69</v>
+        <v>126</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F77" s="10">
         <v>0.11</v>
@@ -2751,16 +2841,16 @@
         <v>25</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>69</v>
+        <v>129</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F78" s="10">
         <v>0.11</v>
@@ -2773,21 +2863,21 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <v>26</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>135</v>
+        <v>69</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F79" s="10">
         <v>0.11</v>
@@ -2805,16 +2895,16 @@
         <v>27</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>139</v>
+        <v>69</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F80" s="10">
         <v>0.11</v>
@@ -2827,21 +2917,21 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <v>28</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D81" s="14" t="s">
-        <v>140</v>
+        <v>119</v>
+      </c>
+      <c r="D81" s="13" t="s">
+        <v>132</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F81" s="10">
         <v>0.11</v>
@@ -2859,16 +2949,16 @@
         <v>29</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F82" s="10">
         <v>0.11</v>
@@ -2886,16 +2976,16 @@
         <v>30</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F83" s="10">
         <v>0.11</v>
@@ -2913,16 +3003,16 @@
         <v>31</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D84" s="13" t="s">
-        <v>71</v>
+        <v>139</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F84" s="10">
         <v>0.11</v>
@@ -2940,16 +3030,16 @@
         <v>32</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D85" s="13" t="s">
-        <v>147</v>
+        <v>119</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>141</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F85" s="10">
         <v>0.11</v>
@@ -2967,16 +3057,16 @@
         <v>33</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D86" s="14" t="s">
-        <v>149</v>
+        <v>119</v>
+      </c>
+      <c r="D86" s="13" t="s">
+        <v>71</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F86" s="10">
         <v>0.11</v>
@@ -2989,21 +3079,21 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
         <v>34</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D87" s="13" t="s">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F87" s="10">
         <v>0.11</v>
@@ -3021,16 +3111,16 @@
         <v>35</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>72</v>
+        <v>146</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F88" s="10">
         <v>0.11</v>
@@ -3043,21 +3133,21 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
         <v>36</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D89" s="13" t="s">
-        <v>153</v>
+        <v>72</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F89" s="10">
         <v>0.11</v>
@@ -3070,21 +3160,21 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
         <v>37</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D90" s="13" t="s">
-        <v>155</v>
+        <v>119</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F90" s="10">
         <v>0.11</v>
@@ -3102,16 +3192,16 @@
         <v>38</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D91" s="13" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F91" s="10">
         <v>0.11</v>
@@ -3124,21 +3214,21 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A92" s="7">
         <v>39</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D92" s="13" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F92" s="10">
         <v>0.11</v>
@@ -3151,225 +3241,401 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="19" t="s">
+    <row r="93" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+      <c r="A93" s="7">
+        <v>40</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D93" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F93" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G93" s="11">
+        <v>1</v>
+      </c>
+      <c r="H93" s="12">
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+      <c r="A94" s="7">
+        <v>41</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D94" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F94" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="G94" s="11">
+        <v>1</v>
+      </c>
+      <c r="H94" s="12">
+        <f t="shared" si="9"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A95" s="7">
+        <v>42</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D95" s="13"/>
+      <c r="E95" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F95" s="10">
+        <v>0.88</v>
+      </c>
+      <c r="G95" s="11">
+        <v>1</v>
+      </c>
+      <c r="H95" s="12">
+        <f t="shared" ref="H95:H104" si="12">F95*G95</f>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A96" s="7">
+        <v>43</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D96" s="13"/>
+      <c r="E96" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F96" s="10">
+        <v>0.22</v>
+      </c>
+      <c r="G96" s="11">
+        <v>1</v>
+      </c>
+      <c r="H96" s="12">
+        <f t="shared" si="12"/>
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="7">
+        <v>44</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D97" s="13"/>
+      <c r="E97" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F97" s="10">
+        <v>0.44</v>
+      </c>
+      <c r="G97" s="11">
+        <v>1</v>
+      </c>
+      <c r="H97" s="12">
+        <f t="shared" si="12"/>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="7">
+        <v>45</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D98" s="13"/>
+      <c r="E98" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F98" s="10">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G98" s="11">
+        <v>1</v>
+      </c>
+      <c r="H98" s="12">
+        <f t="shared" si="12"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A99" s="7">
+        <v>46</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D99" s="13"/>
+      <c r="E99" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F99" s="10">
+        <v>0.54</v>
+      </c>
+      <c r="G99" s="11">
+        <v>1</v>
+      </c>
+      <c r="H99" s="12">
+        <f t="shared" si="12"/>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="7">
+        <v>47</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D100" s="13"/>
+      <c r="E100" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F100" s="10">
+        <v>0.66</v>
+      </c>
+      <c r="G100" s="11">
+        <v>1</v>
+      </c>
+      <c r="H100" s="12">
+        <f t="shared" si="12"/>
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A101" s="7">
+        <v>48</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D101" s="13"/>
+      <c r="E101" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F101" s="10">
+        <v>0.44</v>
+      </c>
+      <c r="G101" s="11">
+        <v>1</v>
+      </c>
+      <c r="H101" s="12">
+        <f t="shared" si="12"/>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A102" s="7">
+        <v>49</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D102" s="13"/>
+      <c r="E102" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F102" s="10">
+        <v>1.21</v>
+      </c>
+      <c r="G102" s="11">
+        <v>1</v>
+      </c>
+      <c r="H102" s="12">
+        <f t="shared" si="12"/>
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A103" s="7">
+        <v>50</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D103" s="13"/>
+      <c r="E103" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="F103" s="10">
+        <v>0.44</v>
+      </c>
+      <c r="G103" s="11">
+        <v>1</v>
+      </c>
+      <c r="H103" s="12">
+        <f t="shared" si="12"/>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A104" s="7">
+        <v>51</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D104" s="13"/>
+      <c r="E104" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F104" s="10">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="G104" s="11">
+        <v>1</v>
+      </c>
+      <c r="H104" s="12">
+        <f t="shared" si="12"/>
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B93" s="20"/>
-      <c r="C93" s="20"/>
-      <c r="D93" s="20"/>
-      <c r="E93" s="20"/>
-      <c r="F93" s="20"/>
-      <c r="G93" s="20"/>
-      <c r="H93" s="21"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="7">
-        <v>1</v>
-      </c>
-      <c r="B94" s="8"/>
-      <c r="C94" s="7"/>
-      <c r="D94" s="13"/>
-      <c r="E94" s="9"/>
-      <c r="F94" s="10"/>
-      <c r="G94" s="11"/>
-      <c r="H94" s="12"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="19" t="s">
+      <c r="B105" s="20"/>
+      <c r="C105" s="20"/>
+      <c r="D105" s="20"/>
+      <c r="E105" s="20"/>
+      <c r="F105" s="20"/>
+      <c r="G105" s="20"/>
+      <c r="H105" s="21"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="7">
+        <v>1</v>
+      </c>
+      <c r="B106" s="8"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="13"/>
+      <c r="E106" s="9"/>
+      <c r="F106" s="10"/>
+      <c r="G106" s="11"/>
+      <c r="H106" s="12"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B95" s="20"/>
-      <c r="C95" s="20"/>
-      <c r="D95" s="20"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="20"/>
-      <c r="G95" s="20"/>
-      <c r="H95" s="21"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="7">
-        <v>1</v>
-      </c>
-      <c r="B96" s="8"/>
-      <c r="C96" s="7"/>
-      <c r="D96" s="13"/>
-      <c r="E96" s="9"/>
-      <c r="F96" s="10"/>
-      <c r="G96" s="11"/>
-      <c r="H96" s="12"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="7">
+      <c r="B107" s="20"/>
+      <c r="C107" s="20"/>
+      <c r="D107" s="20"/>
+      <c r="E107" s="20"/>
+      <c r="F107" s="20"/>
+      <c r="G107" s="20"/>
+      <c r="H107" s="21"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="7">
+        <v>1</v>
+      </c>
+      <c r="B108" s="8"/>
+      <c r="C108" s="7"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="9"/>
+      <c r="F108" s="10"/>
+      <c r="G108" s="11"/>
+      <c r="H108" s="12"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="7">
         <v>2</v>
       </c>
-      <c r="B97" s="8"/>
-      <c r="C97" s="7"/>
-      <c r="D97" s="13"/>
-      <c r="E97" s="9"/>
-      <c r="F97" s="10"/>
-      <c r="G97" s="11"/>
-      <c r="H97" s="12"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="7">
+      <c r="B109" s="8"/>
+      <c r="C109" s="7"/>
+      <c r="D109" s="13"/>
+      <c r="E109" s="9"/>
+      <c r="F109" s="10"/>
+      <c r="G109" s="11"/>
+      <c r="H109" s="12"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="7">
         <v>3</v>
       </c>
-      <c r="B98" s="8"/>
-      <c r="C98" s="7"/>
-      <c r="D98" s="13"/>
-      <c r="E98" s="9"/>
-      <c r="F98" s="10"/>
-      <c r="G98" s="11"/>
-      <c r="H98" s="12"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="16" t="s">
+      <c r="B110" s="8"/>
+      <c r="C110" s="7"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="9"/>
+      <c r="F110" s="10"/>
+      <c r="G110" s="11"/>
+      <c r="H110" s="12"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B99" s="16"/>
-      <c r="C99" s="16"/>
-      <c r="D99" s="16"/>
-      <c r="E99" s="16"/>
-      <c r="F99" s="16"/>
-      <c r="G99" s="16"/>
-      <c r="H99" s="6">
-        <f>SUM(H23:H98)</f>
-        <v>44.169999999999973</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+      <c r="B111" s="16"/>
+      <c r="C111" s="16"/>
+      <c r="D111" s="16"/>
+      <c r="E111" s="16"/>
+      <c r="F111" s="16"/>
+      <c r="G111" s="16"/>
+      <c r="H111" s="6">
+        <f>SUM(H23:H110)</f>
+        <v>49.724999999999952</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B100" s="2"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
-      <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-      <c r="B101" s="2"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
-      <c r="F101" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="G101" s="17"/>
-      <c r="H101" s="17"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-      <c r="B102" s="2"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G102" s="17"/>
-      <c r="H102" s="17"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
-      <c r="B103" s="2"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
-      <c r="E103" s="1"/>
-      <c r="F103" s="1"/>
-      <c r="G103" s="1"/>
-      <c r="H103" s="1"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
-      <c r="B104" s="2"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
-      <c r="G104" s="1"/>
-      <c r="H104" s="1"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
-      <c r="B105" s="2"/>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
-      <c r="E105" s="1"/>
-      <c r="F105" s="1"/>
-      <c r="G105" s="1"/>
-      <c r="H105" s="1"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
-      <c r="B106" s="2"/>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1"/>
-      <c r="E106" s="1"/>
-      <c r="F106" s="1"/>
-      <c r="G106" s="1"/>
-      <c r="H106" s="1"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
-      <c r="B107" s="2"/>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
-      <c r="E107" s="1"/>
-      <c r="F107" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="G107" s="17"/>
-      <c r="H107" s="17"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
-      <c r="B108" s="2"/>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
-      <c r="E108" s="1"/>
-      <c r="F108" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G108" s="17"/>
-      <c r="H108" s="17"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="1"/>
-      <c r="B109" s="2"/>
-      <c r="C109" s="1"/>
-      <c r="D109" s="1"/>
-      <c r="E109" s="1"/>
-      <c r="F109" s="1"/>
-      <c r="G109" s="1"/>
-      <c r="H109" s="1"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
-      <c r="B110" s="2"/>
-      <c r="C110" s="1"/>
-      <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
-      <c r="F110" s="1"/>
-      <c r="G110" s="1"/>
-      <c r="H110" s="1"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
-      <c r="B111" s="2"/>
-      <c r="C111" s="1"/>
-      <c r="D111" s="1"/>
-      <c r="E111" s="1"/>
-      <c r="F111" s="1"/>
-      <c r="G111" s="1"/>
-      <c r="H111" s="1"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
       <c r="B112" s="2"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
@@ -3384,9 +3650,11 @@
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
-      <c r="F113" s="1"/>
-      <c r="G113" s="1"/>
-      <c r="H113" s="1"/>
+      <c r="F113" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G113" s="17"/>
+      <c r="H113" s="17"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
@@ -3394,9 +3662,11 @@
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
-      <c r="F114" s="1"/>
-      <c r="G114" s="1"/>
-      <c r="H114" s="1"/>
+      <c r="F114" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G114" s="17"/>
+      <c r="H114" s="17"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
@@ -3444,9 +3714,11 @@
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
-      <c r="F119" s="1"/>
-      <c r="G119" s="1"/>
-      <c r="H119" s="1"/>
+      <c r="F119" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G119" s="17"/>
+      <c r="H119" s="17"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
@@ -3454,9 +3726,11 @@
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
-      <c r="F120" s="1"/>
-      <c r="G120" s="1"/>
-      <c r="H120" s="1"/>
+      <c r="F120" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G120" s="17"/>
+      <c r="H120" s="17"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
@@ -3608,17 +3882,137 @@
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
     </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="1"/>
+      <c r="B136" s="2"/>
+      <c r="C136" s="1"/>
+      <c r="D136" s="1"/>
+      <c r="E136" s="1"/>
+      <c r="F136" s="1"/>
+      <c r="G136" s="1"/>
+      <c r="H136" s="1"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="1"/>
+      <c r="B137" s="2"/>
+      <c r="C137" s="1"/>
+      <c r="D137" s="1"/>
+      <c r="E137" s="1"/>
+      <c r="F137" s="1"/>
+      <c r="G137" s="1"/>
+      <c r="H137" s="1"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="1"/>
+      <c r="B138" s="2"/>
+      <c r="C138" s="1"/>
+      <c r="D138" s="1"/>
+      <c r="E138" s="1"/>
+      <c r="F138" s="1"/>
+      <c r="G138" s="1"/>
+      <c r="H138" s="1"/>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="1"/>
+      <c r="B139" s="2"/>
+      <c r="C139" s="1"/>
+      <c r="D139" s="1"/>
+      <c r="E139" s="1"/>
+      <c r="F139" s="1"/>
+      <c r="G139" s="1"/>
+      <c r="H139" s="1"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="1"/>
+      <c r="B140" s="2"/>
+      <c r="C140" s="1"/>
+      <c r="D140" s="1"/>
+      <c r="E140" s="1"/>
+      <c r="F140" s="1"/>
+      <c r="G140" s="1"/>
+      <c r="H140" s="1"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" s="1"/>
+      <c r="B141" s="2"/>
+      <c r="C141" s="1"/>
+      <c r="D141" s="1"/>
+      <c r="E141" s="1"/>
+      <c r="F141" s="1"/>
+      <c r="G141" s="1"/>
+      <c r="H141" s="1"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="1"/>
+      <c r="B142" s="2"/>
+      <c r="C142" s="1"/>
+      <c r="D142" s="1"/>
+      <c r="E142" s="1"/>
+      <c r="F142" s="1"/>
+      <c r="G142" s="1"/>
+      <c r="H142" s="1"/>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A143" s="1"/>
+      <c r="B143" s="2"/>
+      <c r="C143" s="1"/>
+      <c r="D143" s="1"/>
+      <c r="E143" s="1"/>
+      <c r="F143" s="1"/>
+      <c r="G143" s="1"/>
+      <c r="H143" s="1"/>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A144" s="1"/>
+      <c r="B144" s="2"/>
+      <c r="C144" s="1"/>
+      <c r="D144" s="1"/>
+      <c r="E144" s="1"/>
+      <c r="F144" s="1"/>
+      <c r="G144" s="1"/>
+      <c r="H144" s="1"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A145" s="1"/>
+      <c r="B145" s="2"/>
+      <c r="C145" s="1"/>
+      <c r="D145" s="1"/>
+      <c r="E145" s="1"/>
+      <c r="F145" s="1"/>
+      <c r="G145" s="1"/>
+      <c r="H145" s="1"/>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A146" s="1"/>
+      <c r="B146" s="2"/>
+      <c r="C146" s="1"/>
+      <c r="D146" s="1"/>
+      <c r="E146" s="1"/>
+      <c r="F146" s="1"/>
+      <c r="G146" s="1"/>
+      <c r="H146" s="1"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147" s="1"/>
+      <c r="B147" s="2"/>
+      <c r="C147" s="1"/>
+      <c r="D147" s="1"/>
+      <c r="E147" s="1"/>
+      <c r="F147" s="1"/>
+      <c r="G147" s="1"/>
+      <c r="H147" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F102:H102"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="F114:H114"/>
+    <mergeCell ref="F119:H119"/>
+    <mergeCell ref="F120:H120"/>
     <mergeCell ref="G19:G20"/>
-    <mergeCell ref="A93:H93"/>
+    <mergeCell ref="A105:H105"/>
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A99:G99"/>
-    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="A111:G111"/>
+    <mergeCell ref="F113:H113"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
@@ -3628,7 +4022,7 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="A39:H39"/>
     <mergeCell ref="A53:H53"/>
-    <mergeCell ref="A95:H95"/>
+    <mergeCell ref="A107:H107"/>
     <mergeCell ref="A24:H24"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
20 maret, sebelum zuhur
</commit_message>
<xml_diff>
--- a/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari - Desember 2021_Debi Tomika.xlsx
+++ b/2021 DEBI TOMIKA/1.Laporan Kegiatan Prakom Januari - Desember 2021_Debi Tomika.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B6DA19-3934-413E-A6A8-A458221E498F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9204DEF7-AA87-4A30-82DA-6C9425D448CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="187">
   <si>
     <t>LAPORAN KEGIATAN PRANATA KOMPUTER</t>
   </si>
@@ -832,6 +832,41 @@
   <si>
     <t>Menyusun Petunjuk Operasional Sistem Informasi Desa Cinta Statistik (SICANTIK)</t>
   </si>
+  <si>
+    <t>Sub Unsur III B Pengolahan Data</t>
+  </si>
+  <si>
+    <t>III.B.7</t>
+  </si>
+  <si>
+    <t>Melakukan Manipulasi Data</t>
+  </si>
+  <si>
+    <r>
+      <t>Melakukan Pemantauan (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Monitoring</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+      </rPr>
+      <t>) Pengolahan Data</t>
+    </r>
+  </si>
+  <si>
+    <t>III.B.6</t>
+  </si>
 </sst>
 </file>
 
@@ -841,7 +876,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -882,6 +917,15 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -897,7 +941,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -957,12 +1001,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1002,12 +1098,6 @@
     <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1022,6 +1112,30 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1304,13 +1418,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H147"/>
+  <dimension ref="A1:V152"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A90" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A96" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="H109" sqref="H109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="34.7109375" style="3" bestFit="1" customWidth="1"/>
@@ -1322,19 +1436,19 @@
     <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
@@ -1344,7 +1458,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1356,7 +1470,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
@@ -1366,7 +1480,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1380,7 +1494,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1394,7 +1508,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1408,7 +1522,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1422,7 +1536,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1436,7 +1550,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="1"/>
@@ -1446,7 +1560,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1458,7 +1572,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1472,7 +1586,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -1486,7 +1600,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1500,7 +1614,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -1514,7 +1628,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -1528,7 +1642,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
@@ -1538,7 +1652,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -1550,45 +1664,45 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+    <row r="19" spans="1:8" ht="42.75">
+      <c r="A19" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="16" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+    <row r="20" spans="1:8">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
       <c r="H20" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
@@ -1614,19 +1728,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+    <row r="22" spans="1:8">
+      <c r="A22" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="21"/>
-    </row>
-    <row r="23" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="19"/>
+    </row>
+    <row r="23" spans="1:8" ht="42.75">
       <c r="A23" s="7">
         <v>1</v>
       </c>
@@ -1653,19 +1767,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+    <row r="24" spans="1:8">
+      <c r="A24" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="21"/>
-    </row>
-    <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="19"/>
+    </row>
+    <row r="25" spans="1:8" ht="42.75">
       <c r="A25" s="7">
         <v>1</v>
       </c>
@@ -1692,7 +1806,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="42.75">
       <c r="A26" s="7">
         <v>2</v>
       </c>
@@ -1719,19 +1833,19 @@
         <v>1.7999999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+    <row r="27" spans="1:8">
+      <c r="A27" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="21"/>
-    </row>
-    <row r="28" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="19"/>
+    </row>
+    <row r="28" spans="1:8" ht="42.75">
       <c r="A28" s="7">
         <v>1</v>
       </c>
@@ -1758,7 +1872,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="42.75">
       <c r="A29" s="7">
         <v>2</v>
       </c>
@@ -1785,7 +1899,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="57">
       <c r="A30" s="7">
         <v>3</v>
       </c>
@@ -1812,7 +1926,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="42.75">
       <c r="A31" s="7">
         <v>4</v>
       </c>
@@ -1839,7 +1953,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="71.25">
       <c r="A32" s="7">
         <v>5</v>
       </c>
@@ -1866,7 +1980,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="71.25">
       <c r="A33" s="7">
         <v>6</v>
       </c>
@@ -1893,7 +2007,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="71.25">
       <c r="A34" s="7">
         <v>7</v>
       </c>
@@ -1920,7 +2034,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="71.25">
       <c r="A35" s="7">
         <v>8</v>
       </c>
@@ -1947,7 +2061,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="42.75">
       <c r="A36" s="7">
         <v>9</v>
       </c>
@@ -1974,7 +2088,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="57">
       <c r="A37" s="7">
         <v>10</v>
       </c>
@@ -2001,7 +2115,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="28.5">
       <c r="A38" s="7">
         <v>11</v>
       </c>
@@ -2028,19 +2142,19 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+    <row r="39" spans="1:8" ht="14.45" customHeight="1">
+      <c r="A39" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="21"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="19"/>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="7">
         <v>1</v>
       </c>
@@ -2052,7 +2166,7 @@
       <c r="G40" s="11"/>
       <c r="H40" s="12"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="7">
         <v>2</v>
       </c>
@@ -2064,7 +2178,7 @@
       <c r="G41" s="11"/>
       <c r="H41" s="12"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="7">
         <v>3</v>
       </c>
@@ -2076,7 +2190,7 @@
       <c r="G42" s="11"/>
       <c r="H42" s="12"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="7">
         <v>4</v>
       </c>
@@ -2088,7 +2202,7 @@
       <c r="G43" s="11"/>
       <c r="H43" s="12"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="7">
         <v>5</v>
       </c>
@@ -2100,7 +2214,7 @@
       <c r="G44" s="11"/>
       <c r="H44" s="12"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="7">
         <v>6</v>
       </c>
@@ -2112,7 +2226,7 @@
       <c r="G45" s="11"/>
       <c r="H45" s="12"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="7">
         <v>7</v>
       </c>
@@ -2124,7 +2238,7 @@
       <c r="G46" s="11"/>
       <c r="H46" s="12"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="7">
         <v>8</v>
       </c>
@@ -2136,7 +2250,7 @@
       <c r="G47" s="11"/>
       <c r="H47" s="12"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="7">
         <v>9</v>
       </c>
@@ -2148,7 +2262,7 @@
       <c r="G48" s="11"/>
       <c r="H48" s="12"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="7">
         <v>10</v>
       </c>
@@ -2160,7 +2274,7 @@
       <c r="G49" s="11"/>
       <c r="H49" s="12"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="7">
         <v>11</v>
       </c>
@@ -2172,7 +2286,7 @@
       <c r="G50" s="11"/>
       <c r="H50" s="12"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="7">
         <v>12</v>
       </c>
@@ -2184,7 +2298,7 @@
       <c r="G51" s="11"/>
       <c r="H51" s="12"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="7">
         <v>13</v>
       </c>
@@ -2196,19 +2310,19 @@
       <c r="G52" s="11"/>
       <c r="H52" s="12"/>
     </row>
-    <row r="53" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
+    <row r="53" spans="1:8" ht="14.45" customHeight="1">
+      <c r="A53" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="21"/>
-    </row>
-    <row r="54" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="19"/>
+    </row>
+    <row r="54" spans="1:8" ht="42.75">
       <c r="A54" s="7">
         <v>1</v>
       </c>
@@ -2235,7 +2349,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="42.75">
       <c r="A55" s="7">
         <v>2</v>
       </c>
@@ -2262,7 +2376,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="42.75">
       <c r="A56" s="7">
         <v>3</v>
       </c>
@@ -2289,7 +2403,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="42.75">
       <c r="A57" s="7">
         <v>4</v>
       </c>
@@ -2316,7 +2430,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="42.75">
       <c r="A58" s="7">
         <v>5</v>
       </c>
@@ -2343,7 +2457,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="42.75">
       <c r="A59" s="7">
         <v>6</v>
       </c>
@@ -2370,7 +2484,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="42.75">
       <c r="A60" s="7">
         <v>7</v>
       </c>
@@ -2397,7 +2511,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="42.75">
       <c r="A61" s="7">
         <v>8</v>
       </c>
@@ -2424,7 +2538,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="42.75">
       <c r="A62" s="7">
         <v>9</v>
       </c>
@@ -2451,7 +2565,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="42.75">
       <c r="A63" s="7">
         <v>10</v>
       </c>
@@ -2478,7 +2592,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="42.75">
       <c r="A64" s="7">
         <v>11</v>
       </c>
@@ -2503,7 +2617,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="42.75">
       <c r="A65" s="7">
         <v>12</v>
       </c>
@@ -2528,7 +2642,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="42.75">
       <c r="A66" s="7">
         <v>13</v>
       </c>
@@ -2553,7 +2667,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="42.75">
       <c r="A67" s="7">
         <v>14</v>
       </c>
@@ -2578,7 +2692,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="42.75">
       <c r="A68" s="7">
         <v>15</v>
       </c>
@@ -2603,7 +2717,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="42.75">
       <c r="A69" s="7">
         <v>16</v>
       </c>
@@ -2628,7 +2742,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="42.75">
       <c r="A70" s="7">
         <v>17</v>
       </c>
@@ -2653,7 +2767,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="42.75">
       <c r="A71" s="7">
         <v>18</v>
       </c>
@@ -2678,7 +2792,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="42.75">
       <c r="A72" s="7">
         <v>19</v>
       </c>
@@ -2703,7 +2817,7 @@
         <v>0.16500000000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="42.75">
       <c r="A73" s="7">
         <v>20</v>
       </c>
@@ -2728,7 +2842,7 @@
         <v>0.16500000000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="57">
       <c r="A74" s="7">
         <v>21</v>
       </c>
@@ -2755,7 +2869,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="57">
       <c r="A75" s="7">
         <v>22</v>
       </c>
@@ -2782,7 +2896,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="57">
       <c r="A76" s="7">
         <v>23</v>
       </c>
@@ -2809,7 +2923,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="57">
       <c r="A77" s="7">
         <v>24</v>
       </c>
@@ -2836,7 +2950,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="57">
       <c r="A78" s="7">
         <v>25</v>
       </c>
@@ -2863,7 +2977,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="71.25">
       <c r="A79" s="7">
         <v>26</v>
       </c>
@@ -2890,7 +3004,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="57">
       <c r="A80" s="7">
         <v>27</v>
       </c>
@@ -2917,7 +3031,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="42.75">
       <c r="A81" s="7">
         <v>28</v>
       </c>
@@ -2944,7 +3058,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="57">
       <c r="A82" s="7">
         <v>29</v>
       </c>
@@ -2971,7 +3085,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="57">
       <c r="A83" s="7">
         <v>30</v>
       </c>
@@ -2998,7 +3112,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="57">
       <c r="A84" s="7">
         <v>31</v>
       </c>
@@ -3025,7 +3139,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="57">
       <c r="A85" s="7">
         <v>32</v>
       </c>
@@ -3052,7 +3166,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="57">
       <c r="A86" s="7">
         <v>33</v>
       </c>
@@ -3079,7 +3193,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="57">
       <c r="A87" s="7">
         <v>34</v>
       </c>
@@ -3106,7 +3220,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="57">
       <c r="A88" s="7">
         <v>35</v>
       </c>
@@ -3133,7 +3247,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="71.25">
       <c r="A89" s="7">
         <v>36</v>
       </c>
@@ -3160,7 +3274,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="57">
       <c r="A90" s="7">
         <v>37</v>
       </c>
@@ -3187,7 +3301,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="57">
       <c r="A91" s="7">
         <v>38</v>
       </c>
@@ -3214,7 +3328,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="71.25">
       <c r="A92" s="7">
         <v>39</v>
       </c>
@@ -3241,7 +3355,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="57">
       <c r="A93" s="7">
         <v>40</v>
       </c>
@@ -3268,7 +3382,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="57">
       <c r="A94" s="7">
         <v>41</v>
       </c>
@@ -3295,7 +3409,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" ht="42.75">
       <c r="A95" s="7">
         <v>42</v>
       </c>
@@ -3320,7 +3434,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="42.75">
       <c r="A96" s="7">
         <v>43</v>
       </c>
@@ -3345,7 +3459,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22" ht="42.75">
       <c r="A97" s="7">
         <v>44</v>
       </c>
@@ -3370,7 +3484,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22" ht="42.75">
       <c r="A98" s="7">
         <v>45</v>
       </c>
@@ -3395,7 +3509,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22" ht="42.75">
       <c r="A99" s="7">
         <v>46</v>
       </c>
@@ -3420,7 +3534,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22" ht="42.75">
       <c r="A100" s="7">
         <v>47</v>
       </c>
@@ -3445,7 +3559,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22" ht="42.75">
       <c r="A101" s="7">
         <v>48</v>
       </c>
@@ -3470,7 +3584,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22" ht="42.75">
       <c r="A102" s="7">
         <v>49</v>
       </c>
@@ -3495,7 +3609,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:22" ht="42.75">
       <c r="A103" s="7">
         <v>50</v>
       </c>
@@ -3520,7 +3634,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:22" ht="42.75">
       <c r="A104" s="7">
         <v>51</v>
       </c>
@@ -3545,151 +3659,287 @@
         <v>0.16500000000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="19" t="s">
+    <row r="105" spans="1:22" ht="14.25" customHeight="1">
+      <c r="A105" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B105" s="23"/>
+      <c r="C105" s="23"/>
+      <c r="D105" s="23"/>
+      <c r="E105" s="23"/>
+      <c r="F105" s="23"/>
+      <c r="G105" s="23"/>
+      <c r="H105" s="24"/>
+      <c r="I105" s="25"/>
+      <c r="J105" s="25"/>
+      <c r="K105" s="25"/>
+      <c r="L105" s="25"/>
+      <c r="M105" s="25"/>
+      <c r="N105" s="25"/>
+      <c r="O105" s="25"/>
+      <c r="P105" s="25"/>
+      <c r="Q105" s="25"/>
+      <c r="R105" s="25"/>
+      <c r="S105" s="25"/>
+      <c r="T105" s="25"/>
+      <c r="U105" s="25"/>
+      <c r="V105" s="25"/>
+    </row>
+    <row r="106" spans="1:22" ht="35.25" customHeight="1">
+      <c r="A106" s="26">
+        <v>1</v>
+      </c>
+      <c r="B106" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="C106" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="D106" s="26">
+        <v>2021</v>
+      </c>
+      <c r="E106" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F106" s="26">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="G106" s="26">
+        <v>18</v>
+      </c>
+      <c r="H106" s="26">
+        <f>F106*G106</f>
+        <v>2.97</v>
+      </c>
+      <c r="I106" s="25"/>
+      <c r="J106" s="25"/>
+      <c r="K106" s="25"/>
+      <c r="L106" s="25"/>
+      <c r="M106" s="25"/>
+      <c r="N106" s="25"/>
+      <c r="O106" s="25"/>
+      <c r="P106" s="25"/>
+      <c r="Q106" s="25"/>
+      <c r="R106" s="25"/>
+      <c r="S106" s="25"/>
+      <c r="T106" s="25"/>
+      <c r="U106" s="25"/>
+      <c r="V106" s="25"/>
+    </row>
+    <row r="107" spans="1:22" ht="35.25" customHeight="1">
+      <c r="A107" s="26">
+        <v>2</v>
+      </c>
+      <c r="B107" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="C107" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="D107" s="26">
+        <v>2021</v>
+      </c>
+      <c r="E107" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F107" s="26">
+        <v>0.08</v>
+      </c>
+      <c r="G107" s="26">
+        <v>52</v>
+      </c>
+      <c r="H107" s="26">
+        <f>F107*G107</f>
+        <v>4.16</v>
+      </c>
+      <c r="I107" s="25"/>
+      <c r="J107" s="25"/>
+      <c r="K107" s="25"/>
+      <c r="L107" s="25"/>
+      <c r="M107" s="25"/>
+      <c r="N107" s="25"/>
+      <c r="O107" s="25"/>
+      <c r="P107" s="25"/>
+      <c r="Q107" s="25"/>
+      <c r="R107" s="25"/>
+      <c r="S107" s="25"/>
+      <c r="T107" s="25"/>
+      <c r="U107" s="25"/>
+      <c r="V107" s="25"/>
+    </row>
+    <row r="108" spans="1:22" ht="35.25" customHeight="1">
+      <c r="A108" s="26">
+        <v>3</v>
+      </c>
+      <c r="B108" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="C108" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="D108" s="26">
+        <v>2022</v>
+      </c>
+      <c r="E108" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F108" s="26">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="G108" s="26">
+        <v>18</v>
+      </c>
+      <c r="H108" s="26">
+        <f>F108*G108</f>
+        <v>2.97</v>
+      </c>
+      <c r="I108" s="25"/>
+      <c r="J108" s="25"/>
+      <c r="K108" s="25"/>
+      <c r="L108" s="25"/>
+      <c r="M108" s="25"/>
+      <c r="N108" s="25"/>
+      <c r="O108" s="25"/>
+      <c r="P108" s="25"/>
+      <c r="Q108" s="25"/>
+      <c r="R108" s="25"/>
+      <c r="S108" s="25"/>
+      <c r="T108" s="25"/>
+      <c r="U108" s="25"/>
+      <c r="V108" s="25"/>
+    </row>
+    <row r="109" spans="1:22" ht="35.25" customHeight="1">
+      <c r="A109" s="26">
+        <v>4</v>
+      </c>
+      <c r="B109" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="C109" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="D109" s="26">
+        <v>2022</v>
+      </c>
+      <c r="E109" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F109" s="26">
+        <v>0.08</v>
+      </c>
+      <c r="G109" s="26">
+        <v>52</v>
+      </c>
+      <c r="H109" s="26">
+        <f>F109*G109</f>
+        <v>4.16</v>
+      </c>
+      <c r="I109" s="25"/>
+      <c r="J109" s="25"/>
+      <c r="K109" s="25"/>
+      <c r="L109" s="25"/>
+      <c r="M109" s="25"/>
+      <c r="N109" s="25"/>
+      <c r="O109" s="25"/>
+      <c r="P109" s="25"/>
+      <c r="Q109" s="25"/>
+      <c r="R109" s="25"/>
+      <c r="S109" s="25"/>
+      <c r="T109" s="25"/>
+      <c r="U109" s="25"/>
+      <c r="V109" s="25"/>
+    </row>
+    <row r="110" spans="1:22" ht="15" customHeight="1">
+      <c r="A110" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B105" s="20"/>
-      <c r="C105" s="20"/>
-      <c r="D105" s="20"/>
-      <c r="E105" s="20"/>
-      <c r="F105" s="20"/>
-      <c r="G105" s="20"/>
-      <c r="H105" s="21"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="7">
-        <v>1</v>
-      </c>
-      <c r="B106" s="8"/>
-      <c r="C106" s="7"/>
-      <c r="D106" s="13"/>
-      <c r="E106" s="9"/>
-      <c r="F106" s="10"/>
-      <c r="G106" s="11"/>
-      <c r="H106" s="12"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="19" t="s">
+      <c r="B110" s="18"/>
+      <c r="C110" s="18"/>
+      <c r="D110" s="18"/>
+      <c r="E110" s="18"/>
+      <c r="F110" s="18"/>
+      <c r="G110" s="18"/>
+      <c r="H110" s="19"/>
+    </row>
+    <row r="111" spans="1:22">
+      <c r="A111" s="7">
+        <v>1</v>
+      </c>
+      <c r="B111" s="8"/>
+      <c r="C111" s="7"/>
+      <c r="D111" s="13"/>
+      <c r="E111" s="9"/>
+      <c r="F111" s="10"/>
+      <c r="G111" s="11"/>
+      <c r="H111" s="12"/>
+    </row>
+    <row r="112" spans="1:22">
+      <c r="A112" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B107" s="20"/>
-      <c r="C107" s="20"/>
-      <c r="D107" s="20"/>
-      <c r="E107" s="20"/>
-      <c r="F107" s="20"/>
-      <c r="G107" s="20"/>
-      <c r="H107" s="21"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="7">
-        <v>1</v>
-      </c>
-      <c r="B108" s="8"/>
-      <c r="C108" s="7"/>
-      <c r="D108" s="13"/>
-      <c r="E108" s="9"/>
-      <c r="F108" s="10"/>
-      <c r="G108" s="11"/>
-      <c r="H108" s="12"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="7">
+      <c r="B112" s="18"/>
+      <c r="C112" s="18"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="18"/>
+      <c r="F112" s="18"/>
+      <c r="G112" s="18"/>
+      <c r="H112" s="19"/>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="A113" s="7">
+        <v>1</v>
+      </c>
+      <c r="B113" s="8"/>
+      <c r="C113" s="7"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="9"/>
+      <c r="F113" s="10"/>
+      <c r="G113" s="11"/>
+      <c r="H113" s="12"/>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114" s="7">
         <v>2</v>
       </c>
-      <c r="B109" s="8"/>
-      <c r="C109" s="7"/>
-      <c r="D109" s="13"/>
-      <c r="E109" s="9"/>
-      <c r="F109" s="10"/>
-      <c r="G109" s="11"/>
-      <c r="H109" s="12"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="7">
+      <c r="B114" s="8"/>
+      <c r="C114" s="7"/>
+      <c r="D114" s="13"/>
+      <c r="E114" s="9"/>
+      <c r="F114" s="10"/>
+      <c r="G114" s="11"/>
+      <c r="H114" s="12"/>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" s="7">
         <v>3</v>
       </c>
-      <c r="B110" s="8"/>
-      <c r="C110" s="7"/>
-      <c r="D110" s="13"/>
-      <c r="E110" s="9"/>
-      <c r="F110" s="10"/>
-      <c r="G110" s="11"/>
-      <c r="H110" s="12"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="16" t="s">
+      <c r="B115" s="8"/>
+      <c r="C115" s="7"/>
+      <c r="D115" s="13"/>
+      <c r="E115" s="9"/>
+      <c r="F115" s="10"/>
+      <c r="G115" s="11"/>
+      <c r="H115" s="12"/>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B111" s="16"/>
-      <c r="C111" s="16"/>
-      <c r="D111" s="16"/>
-      <c r="E111" s="16"/>
-      <c r="F111" s="16"/>
-      <c r="G111" s="16"/>
-      <c r="H111" s="6">
-        <f>SUM(H23:H110)</f>
-        <v>49.724999999999952</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+      <c r="B116" s="21"/>
+      <c r="C116" s="21"/>
+      <c r="D116" s="21"/>
+      <c r="E116" s="21"/>
+      <c r="F116" s="21"/>
+      <c r="G116" s="21"/>
+      <c r="H116" s="6">
+        <f>SUM(H23:H115)</f>
+        <v>63.984999999999943</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B112" s="2"/>
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-      <c r="E112" s="1"/>
-      <c r="F112" s="1"/>
-      <c r="G112" s="1"/>
-      <c r="H112" s="1"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
-      <c r="B113" s="2"/>
-      <c r="C113" s="1"/>
-      <c r="D113" s="1"/>
-      <c r="E113" s="1"/>
-      <c r="F113" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="G113" s="17"/>
-      <c r="H113" s="17"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-      <c r="B114" s="2"/>
-      <c r="C114" s="1"/>
-      <c r="D114" s="1"/>
-      <c r="E114" s="1"/>
-      <c r="F114" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G114" s="17"/>
-      <c r="H114" s="17"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
-      <c r="B115" s="2"/>
-      <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
-      <c r="E115" s="1"/>
-      <c r="F115" s="1"/>
-      <c r="G115" s="1"/>
-      <c r="H115" s="1"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
-      <c r="B116" s="2"/>
-      <c r="C116" s="1"/>
-      <c r="D116" s="1"/>
-      <c r="E116" s="1"/>
-      <c r="F116" s="1"/>
-      <c r="G116" s="1"/>
-      <c r="H116" s="1"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
       <c r="B117" s="2"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
@@ -3698,41 +3948,41 @@
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8">
       <c r="A118" s="1"/>
       <c r="B118" s="2"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
-      <c r="F118" s="1"/>
-      <c r="G118" s="1"/>
-      <c r="H118" s="1"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F118" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G118" s="15"/>
+      <c r="H118" s="15"/>
+    </row>
+    <row r="119" spans="1:8">
       <c r="A119" s="1"/>
       <c r="B119" s="2"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
-      <c r="F119" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="G119" s="17"/>
-      <c r="H119" s="17"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F119" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G119" s="15"/>
+      <c r="H119" s="15"/>
+    </row>
+    <row r="120" spans="1:8">
       <c r="A120" s="1"/>
       <c r="B120" s="2"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
-      <c r="F120" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G120" s="17"/>
-      <c r="H120" s="17"/>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
+      <c r="H120" s="1"/>
+    </row>
+    <row r="121" spans="1:8">
       <c r="A121" s="1"/>
       <c r="B121" s="2"/>
       <c r="C121" s="1"/>
@@ -3742,7 +3992,7 @@
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8">
       <c r="A122" s="1"/>
       <c r="B122" s="2"/>
       <c r="C122" s="1"/>
@@ -3752,7 +4002,7 @@
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8">
       <c r="A123" s="1"/>
       <c r="B123" s="2"/>
       <c r="C123" s="1"/>
@@ -3762,27 +4012,31 @@
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8">
       <c r="A124" s="1"/>
       <c r="B124" s="2"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
-      <c r="F124" s="1"/>
-      <c r="G124" s="1"/>
-      <c r="H124" s="1"/>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F124" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G124" s="15"/>
+      <c r="H124" s="15"/>
+    </row>
+    <row r="125" spans="1:8">
       <c r="A125" s="1"/>
       <c r="B125" s="2"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
-      <c r="F125" s="1"/>
-      <c r="G125" s="1"/>
-      <c r="H125" s="1"/>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F125" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G125" s="15"/>
+      <c r="H125" s="15"/>
+    </row>
+    <row r="126" spans="1:8">
       <c r="A126" s="1"/>
       <c r="B126" s="2"/>
       <c r="C126" s="1"/>
@@ -3792,7 +4046,7 @@
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8">
       <c r="A127" s="1"/>
       <c r="B127" s="2"/>
       <c r="C127" s="1"/>
@@ -3802,7 +4056,7 @@
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8">
       <c r="A128" s="1"/>
       <c r="B128" s="2"/>
       <c r="C128" s="1"/>
@@ -3812,7 +4066,7 @@
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8">
       <c r="A129" s="1"/>
       <c r="B129" s="2"/>
       <c r="C129" s="1"/>
@@ -3822,7 +4076,7 @@
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8">
       <c r="A130" s="1"/>
       <c r="B130" s="2"/>
       <c r="C130" s="1"/>
@@ -3832,7 +4086,7 @@
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8">
       <c r="A131" s="1"/>
       <c r="B131" s="2"/>
       <c r="C131" s="1"/>
@@ -3842,7 +4096,7 @@
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8">
       <c r="A132" s="1"/>
       <c r="B132" s="2"/>
       <c r="C132" s="1"/>
@@ -3852,7 +4106,7 @@
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8">
       <c r="A133" s="1"/>
       <c r="B133" s="2"/>
       <c r="C133" s="1"/>
@@ -3862,7 +4116,7 @@
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8">
       <c r="A134" s="1"/>
       <c r="B134" s="2"/>
       <c r="C134" s="1"/>
@@ -3872,7 +4126,7 @@
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8">
       <c r="A135" s="1"/>
       <c r="B135" s="2"/>
       <c r="C135" s="1"/>
@@ -3882,7 +4136,7 @@
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8">
       <c r="A136" s="1"/>
       <c r="B136" s="2"/>
       <c r="C136" s="1"/>
@@ -3892,7 +4146,7 @@
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8">
       <c r="A137" s="1"/>
       <c r="B137" s="2"/>
       <c r="C137" s="1"/>
@@ -3902,7 +4156,7 @@
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8">
       <c r="A138" s="1"/>
       <c r="B138" s="2"/>
       <c r="C138" s="1"/>
@@ -3912,7 +4166,7 @@
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8">
       <c r="A139" s="1"/>
       <c r="B139" s="2"/>
       <c r="C139" s="1"/>
@@ -3922,7 +4176,7 @@
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8">
       <c r="A140" s="1"/>
       <c r="B140" s="2"/>
       <c r="C140" s="1"/>
@@ -3932,7 +4186,7 @@
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8">
       <c r="A141" s="1"/>
       <c r="B141" s="2"/>
       <c r="C141" s="1"/>
@@ -3942,7 +4196,7 @@
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8">
       <c r="A142" s="1"/>
       <c r="B142" s="2"/>
       <c r="C142" s="1"/>
@@ -3952,7 +4206,7 @@
       <c r="G142" s="1"/>
       <c r="H142" s="1"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8">
       <c r="A143" s="1"/>
       <c r="B143" s="2"/>
       <c r="C143" s="1"/>
@@ -3962,7 +4216,7 @@
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8">
       <c r="A144" s="1"/>
       <c r="B144" s="2"/>
       <c r="C144" s="1"/>
@@ -3972,7 +4226,7 @@
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8">
       <c r="A145" s="1"/>
       <c r="B145" s="2"/>
       <c r="C145" s="1"/>
@@ -3982,7 +4236,7 @@
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8">
       <c r="A146" s="1"/>
       <c r="B146" s="2"/>
       <c r="C146" s="1"/>
@@ -3992,7 +4246,7 @@
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8">
       <c r="A147" s="1"/>
       <c r="B147" s="2"/>
       <c r="C147" s="1"/>
@@ -4002,17 +4256,61 @@
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
     </row>
+    <row r="148" spans="1:8">
+      <c r="A148" s="1"/>
+      <c r="B148" s="2"/>
+      <c r="C148" s="1"/>
+      <c r="D148" s="1"/>
+      <c r="E148" s="1"/>
+      <c r="F148" s="1"/>
+      <c r="G148" s="1"/>
+      <c r="H148" s="1"/>
+    </row>
+    <row r="149" spans="1:8">
+      <c r="A149" s="1"/>
+      <c r="B149" s="2"/>
+      <c r="C149" s="1"/>
+      <c r="D149" s="1"/>
+      <c r="E149" s="1"/>
+      <c r="F149" s="1"/>
+      <c r="G149" s="1"/>
+      <c r="H149" s="1"/>
+    </row>
+    <row r="150" spans="1:8">
+      <c r="A150" s="1"/>
+      <c r="B150" s="2"/>
+      <c r="C150" s="1"/>
+      <c r="D150" s="1"/>
+      <c r="E150" s="1"/>
+      <c r="F150" s="1"/>
+      <c r="G150" s="1"/>
+      <c r="H150" s="1"/>
+    </row>
+    <row r="151" spans="1:8">
+      <c r="A151" s="1"/>
+      <c r="B151" s="2"/>
+      <c r="C151" s="1"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1"/>
+      <c r="F151" s="1"/>
+      <c r="G151" s="1"/>
+      <c r="H151" s="1"/>
+    </row>
+    <row r="152" spans="1:8">
+      <c r="A152" s="1"/>
+      <c r="B152" s="2"/>
+      <c r="C152" s="1"/>
+      <c r="D152" s="1"/>
+      <c r="E152" s="1"/>
+      <c r="F152" s="1"/>
+      <c r="G152" s="1"/>
+      <c r="H152" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="F114:H114"/>
-    <mergeCell ref="F119:H119"/>
-    <mergeCell ref="F120:H120"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="A105:H105"/>
-    <mergeCell ref="A22:H22"/>
+  <mergeCells count="21">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A111:G111"/>
-    <mergeCell ref="F113:H113"/>
+    <mergeCell ref="A116:G116"/>
+    <mergeCell ref="F118:H118"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
@@ -4022,8 +4320,15 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="A39:H39"/>
     <mergeCell ref="A53:H53"/>
-    <mergeCell ref="A107:H107"/>
+    <mergeCell ref="A112:H112"/>
     <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A105:H105"/>
+    <mergeCell ref="F119:H119"/>
+    <mergeCell ref="F124:H124"/>
+    <mergeCell ref="F125:H125"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="A110:H110"/>
+    <mergeCell ref="A22:H22"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>